<commit_message>
2023 July 24 01:09pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/One Model/Correlations/correlations fed.xlsx
+++ b/Models/Fed Models/One Model/Correlations/correlations fed.xlsx
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5083</v>
+        <v>0.5327</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5947</v>
+        <v>0.6011</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5232</v>
+        <v>0.2799</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5848</v>
+        <v>0.4121</v>
       </c>
     </row>
     <row r="6">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4288</v>
+        <v>-0.1786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed data for SP500 to Yahoo Finance
</commit_message>
<xml_diff>
--- a/Models/Fed Models/One Model/Correlations/correlations fed.xlsx
+++ b/Models/Fed Models/One Model/Correlations/correlations fed.xlsx
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5397</v>
+        <v>0.6516</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6303</v>
+        <v>0.7111</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3131</v>
+        <v>0.3024</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4133</v>
+        <v>0.4279</v>
       </c>
     </row>
     <row r="6">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.1845</v>
+        <v>-0.1396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>